<commit_message>
situacini done dashnia done
</commit_message>
<xml_diff>
--- a/3-Katet/regjistri/29-Koordinatat-e-kateve-953-5-TalJer-Faruki-leg.xlsx
+++ b/3-Katet/regjistri/29-Koordinatat-e-kateve-953-5-TalJer-Faruki-leg.xlsx
@@ -1,39 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Ferizaj\Greme\Ingjinjerike\173-4-Greme-Ademi\3-Katet\regjistri\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ferizaj\Talinoc-i-Jerlive\INXHINIERIKE\513-4-Agimi-legalizim\ob1\3-Katet\regjistri\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AFB2CE-5F3E-41D3-901C-BF6C132C146B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="1005" yWindow="195" windowWidth="27795" windowHeight="16005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$49</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$48</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="23">
   <si>
     <t>Y</t>
   </si>
@@ -81,31 +76,37 @@
     <t>Gjithsej:</t>
   </si>
   <si>
+    <t>Liridon Sejdiu</t>
+  </si>
+  <si>
     <t>Terasa</t>
   </si>
   <si>
-    <t>PERDHESA</t>
-  </si>
-  <si>
-    <t>Liridon Sejdiu</t>
-  </si>
-  <si>
-    <t>PERDHESA-TERAS</t>
-  </si>
-  <si>
-    <t>KATI1</t>
-  </si>
-  <si>
-    <t>KATI1-TERASA</t>
-  </si>
-  <si>
     <t>Kati 1</t>
+  </si>
+  <si>
+    <t>perdhese</t>
+  </si>
+  <si>
+    <t>kati1</t>
+  </si>
+  <si>
+    <t>perdhesa</t>
+  </si>
+  <si>
+    <t>bodrum</t>
+  </si>
+  <si>
+    <t>Bodrumi</t>
+  </si>
+  <si>
+    <t>kati1-terasa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -147,7 +148,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -424,11 +425,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -439,33 +591,143 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -479,80 +741,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -716,7 +912,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5852594" y="2351539"/>
+          <a:off x="5426340" y="2343781"/>
           <a:ext cx="2953749" cy="298800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -749,7 +945,7 @@
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>Zona Kadastrale: Greme</a:t>
+            <a:t>Zona Kadastrale: Talinoc i Jerlive</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -824,7 +1020,7 @@
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>: 00173-4</a:t>
+            <a:t>: 00513-4</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1191,19 +1387,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="I33" sqref="B26:I33"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="E33" sqref="B29:I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
     <col min="8" max="8" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" customWidth="1"/>
@@ -1211,115 +1408,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34"/>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
     </row>
     <row r="4" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="35"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="37"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="24"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="38"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="40"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="27"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="41"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="43"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="30"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D12" s="4"/>
@@ -1329,604 +1526,643 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="11">
-        <v>9</v>
+      <c r="B15" s="12">
+        <v>210</v>
       </c>
       <c r="C15" s="5">
-        <v>7512915.9336999999</v>
+        <v>7513383.4850000003</v>
       </c>
       <c r="D15" s="5">
-        <v>4688194.9045000002</v>
-      </c>
-      <c r="E15" s="10">
-        <v>601.94100000000003</v>
-      </c>
-      <c r="F15" s="10" t="s">
+        <v>4694172.0411</v>
+      </c>
+      <c r="E15" s="13">
+        <v>619.96699999999998</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" s="34">
+        <v>85.68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="12">
+        <v>206</v>
+      </c>
+      <c r="C16" s="5">
+        <v>7513387.5690000001</v>
+      </c>
+      <c r="D16" s="5">
+        <v>4694163.568</v>
+      </c>
+      <c r="E16" s="13">
+        <v>619.96699999999998</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="35"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="12">
+        <v>207</v>
+      </c>
+      <c r="C17" s="5">
+        <v>7513379.3870000001</v>
+      </c>
+      <c r="D17" s="5">
+        <v>4694159.5640000002</v>
+      </c>
+      <c r="E17" s="13">
+        <v>619.96699999999998</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="35"/>
+    </row>
+    <row r="18" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="12">
+        <v>209</v>
+      </c>
+      <c r="C18" s="5">
+        <v>7513375.3048</v>
+      </c>
+      <c r="D18" s="5">
+        <v>4694168.0379999997</v>
+      </c>
+      <c r="E18" s="13">
+        <v>619.96699999999998</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="33"/>
+      <c r="H18" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="15">
+        <f>SUM(I15:I17)</f>
+        <v>85.68</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+    </row>
+    <row r="20" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="12">
+        <v>218</v>
+      </c>
+      <c r="C22" s="5">
+        <v>7513374.3994000005</v>
+      </c>
+      <c r="D22" s="5">
+        <v>4694167.5948999999</v>
+      </c>
+      <c r="E22" s="13">
+        <v>617.26700000000005</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="20">
+        <v>87.6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="12">
+        <v>219</v>
+      </c>
+      <c r="C23" s="5">
+        <v>7513375.2303999998</v>
+      </c>
+      <c r="D23" s="5">
+        <v>4694165.8744000001</v>
+      </c>
+      <c r="E23" s="13">
+        <v>617.26700000000005</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="50"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="20"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="12">
+        <v>220</v>
+      </c>
+      <c r="C24" s="5">
+        <v>7513376.1339999996</v>
+      </c>
+      <c r="D24" s="5">
+        <v>4694166.3165999996</v>
+      </c>
+      <c r="E24" s="13">
+        <v>617.26700000000005</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="50"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="20"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="12">
+        <v>221</v>
+      </c>
+      <c r="C25" s="5">
+        <v>7513383.4850000003</v>
+      </c>
+      <c r="D25" s="5">
+        <v>4694172.0411</v>
+      </c>
+      <c r="E25" s="13">
+        <v>617.26700000000005</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" s="50"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="20"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="12">
+        <v>222</v>
+      </c>
+      <c r="C26" s="5">
+        <v>7513379.3870000001</v>
+      </c>
+      <c r="D26" s="5">
+        <v>4694159.5640000002</v>
+      </c>
+      <c r="E26" s="13">
+        <v>617.26700000000005</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" s="50"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="20"/>
+    </row>
+    <row r="27" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="12">
+        <v>224</v>
+      </c>
+      <c r="C27" s="5">
+        <v>7513387.5609999998</v>
+      </c>
+      <c r="D27" s="5">
+        <v>4694163.5640000002</v>
+      </c>
+      <c r="E27" s="13">
+        <v>617.26700000000005</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="51"/>
+      <c r="H27" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" s="15">
+        <f>SUM(I22:I26)</f>
+        <v>87.6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="6"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="12">
+        <v>211</v>
+      </c>
+      <c r="C30" s="5">
+        <v>7513375.3048</v>
+      </c>
+      <c r="D30" s="5">
+        <v>4694168.0379999997</v>
+      </c>
+      <c r="E30" s="13">
+        <v>623.09100000000001</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="20">
+        <v>90.435000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="12">
+        <v>212</v>
+      </c>
+      <c r="C31" s="5">
+        <v>7513383.4850000003</v>
+      </c>
+      <c r="D31" s="5">
+        <v>4694172.0411</v>
+      </c>
+      <c r="E31" s="13">
+        <v>623.09100000000001</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="50"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="20"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="12">
+        <v>213</v>
+      </c>
+      <c r="C32" s="5">
+        <v>7513377.3195000002</v>
+      </c>
+      <c r="D32" s="5">
+        <v>4694163.8557000002</v>
+      </c>
+      <c r="E32" s="13">
+        <v>623.09100000000001</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" s="50"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="20"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="12">
+        <v>214</v>
+      </c>
+      <c r="C33" s="5">
+        <v>7513378.4885</v>
+      </c>
+      <c r="D33" s="5">
+        <v>4694159.1243000003</v>
+      </c>
+      <c r="E33" s="13">
+        <v>623.09100000000001</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" s="50"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="20"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B34" s="12">
+        <v>215</v>
+      </c>
+      <c r="C34" s="5">
+        <v>7513387.5690000001</v>
+      </c>
+      <c r="D34" s="5">
+        <v>4694163.568</v>
+      </c>
+      <c r="E34" s="13">
+        <v>623.09100000000001</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="50"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="20"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B35" s="12">
+        <v>216</v>
+      </c>
+      <c r="C35" s="5">
+        <v>7513376.4210000001</v>
+      </c>
+      <c r="D35" s="5">
+        <v>4694163.4160000002</v>
+      </c>
+      <c r="E35" s="13">
+        <v>623.09100000000001</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" s="50"/>
+      <c r="H35" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="I15" s="44">
-        <v>72.028000000000006</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="11">
-        <v>10</v>
-      </c>
-      <c r="C16" s="5">
-        <v>7512912.4574999996</v>
-      </c>
-      <c r="D16" s="5">
-        <v>4688193.57</v>
-      </c>
-      <c r="E16" s="10">
-        <v>601.94100000000003</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="44"/>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="11">
-        <v>11</v>
-      </c>
-      <c r="C17" s="5">
-        <v>7512912.7120000003</v>
-      </c>
-      <c r="D17" s="5">
-        <v>4688192.9069999997</v>
-      </c>
-      <c r="E17" s="10">
-        <v>601.94100000000003</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="11">
-        <v>14</v>
-      </c>
-      <c r="C18" s="5">
-        <v>7512908.3671000004</v>
-      </c>
-      <c r="D18" s="5">
-        <v>4688191.2390000001</v>
-      </c>
-      <c r="E18" s="10">
-        <v>601.94100000000003</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="44"/>
-      <c r="M18">
-        <v>78.774000000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="11">
-        <v>15</v>
-      </c>
-      <c r="C19" s="5">
-        <v>7512905.0319999997</v>
-      </c>
-      <c r="D19" s="5">
-        <v>4688199.3990000002</v>
-      </c>
-      <c r="E19" s="10">
-        <v>601.94100000000003</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
-      <c r="M19">
-        <v>4.4909999999999997</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="11">
-        <v>167</v>
-      </c>
-      <c r="C20" s="5">
-        <v>7512912.8032999998</v>
-      </c>
-      <c r="D20" s="5">
-        <v>4688202.5635000002</v>
-      </c>
-      <c r="E20" s="10">
-        <v>601.94100000000003</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="44"/>
-      <c r="M20">
-        <f>SUM(M18:M19)</f>
-        <v>83.265000000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="11">
-        <v>7</v>
-      </c>
-      <c r="C21" s="5">
-        <v>7512916.9979999997</v>
-      </c>
-      <c r="D21" s="5">
-        <v>4688192.1320000002</v>
-      </c>
-      <c r="E21" s="10">
-        <v>601.94100000000003</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="44"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="11">
-        <v>12</v>
-      </c>
-      <c r="C22" s="5">
-        <v>7512911.5231999997</v>
-      </c>
-      <c r="D22" s="5">
-        <v>4688192.4506000001</v>
-      </c>
-      <c r="E22" s="10">
-        <v>601.94100000000003</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" s="44"/>
-      <c r="H22" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22" s="10">
-        <v>14.036</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="11">
+      <c r="I35" s="20">
+        <v>4.6609999999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="56">
+        <v>217</v>
+      </c>
+      <c r="C36" s="57">
+        <v>7513374.3994000005</v>
+      </c>
+      <c r="D36" s="57">
+        <v>4694167.5948999999</v>
+      </c>
+      <c r="E36" s="14">
+        <v>623.09100000000001</v>
+      </c>
+      <c r="F36" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36" s="51"/>
+      <c r="H36" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="5">
-        <v>7512912.3669999996</v>
-      </c>
-      <c r="D23" s="5">
-        <v>4688190.3370000003</v>
-      </c>
-      <c r="E23" s="10">
-        <v>601.94100000000003</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="44"/>
-      <c r="H23" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I23" s="15">
-        <f>SUM(I15:I22)</f>
-        <v>86.064000000000007</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D25" s="6"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G26" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H26" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="I26" s="14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="11">
-        <v>26</v>
-      </c>
-      <c r="C27" s="5">
-        <v>7512912.8032999998</v>
-      </c>
-      <c r="D27" s="5">
-        <v>4688202.5635000002</v>
-      </c>
-      <c r="E27" s="10">
-        <v>604.78599999999994</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G27" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="H27" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="I27" s="44">
-        <v>78.774000000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="11">
-        <v>27</v>
-      </c>
-      <c r="C28" s="5">
-        <v>7512912.7340000002</v>
-      </c>
-      <c r="D28" s="5">
-        <v>4688191.807</v>
-      </c>
-      <c r="E28" s="10">
-        <v>604.78599999999994</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="44"/>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="11">
-        <v>28</v>
-      </c>
-      <c r="C29" s="5">
-        <v>7512912.3449999997</v>
-      </c>
-      <c r="D29" s="5">
-        <v>4688192.7699999996</v>
-      </c>
-      <c r="E29" s="10">
-        <v>604.78599999999994</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="11">
-        <v>29</v>
-      </c>
-      <c r="C30" s="5">
-        <v>7512908.3671000004</v>
-      </c>
-      <c r="D30" s="5">
-        <v>4688191.2390000001</v>
-      </c>
-      <c r="E30" s="10">
-        <v>604.78599999999994</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="11">
-        <v>30</v>
-      </c>
-      <c r="C31" s="5">
-        <v>7512905.0429999996</v>
-      </c>
-      <c r="D31" s="5">
-        <v>4688199.4000000004</v>
-      </c>
-      <c r="E31" s="10">
-        <v>604.78599999999994</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G31" s="44"/>
-      <c r="H31" s="44"/>
-      <c r="I31" s="44"/>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="11">
-        <v>31</v>
-      </c>
-      <c r="C32" s="5">
-        <v>7512916.5610999996</v>
-      </c>
-      <c r="D32" s="5">
-        <v>4688193.3693000004</v>
-      </c>
-      <c r="E32" s="10">
-        <v>604.78599999999994</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G32" s="44"/>
-      <c r="H32" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I32" s="10">
-        <v>4.4909999999999997</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B33" s="11">
-        <v>25</v>
-      </c>
-      <c r="C33" s="5">
-        <v>7512908.7709999997</v>
-      </c>
-      <c r="D33" s="5">
-        <v>4688190.2439999999</v>
-      </c>
-      <c r="E33" s="10">
-        <v>604.78599999999994</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G33" s="44"/>
-      <c r="H33" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I33" s="15">
-        <f>SUM(I27:I32)</f>
-        <v>83.265000000000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D34" s="6"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D35" s="6"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D36" s="6"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
+      <c r="I36" s="15">
+        <f>SUM(I30:I35)</f>
+        <v>95.096000000000004</v>
+      </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D37" s="6"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="19"/>
       <c r="G37" s="8"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D38" s="6"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="19"/>
       <c r="G38" s="8"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D39" s="6"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="19"/>
       <c r="G39" s="8"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D40" s="6"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="19"/>
       <c r="G40" s="8"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D41" s="6"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="19"/>
       <c r="G41" s="8"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D42" s="6"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="19"/>
       <c r="G42" s="8"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D43" s="6"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="19"/>
       <c r="G43" s="8"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="18"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D44" s="6"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="19"/>
       <c r="G44" s="8"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="18"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D45" s="6"/>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
       <c r="G45" s="8"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="9"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
-    </row>
-    <row r="47" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K47" s="1"/>
-    </row>
-    <row r="48" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+    </row>
+    <row r="46" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K46" s="1"/>
+    </row>
+    <row r="47" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="F48" s="26"/>
-      <c r="G48" s="27"/>
-      <c r="H48" s="21" t="s">
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47" s="42"/>
+      <c r="G47" s="43"/>
+      <c r="H47" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="I48" s="22"/>
-      <c r="J48" s="16"/>
-      <c r="K48" s="17"/>
-    </row>
-    <row r="49" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="28" t="s">
+      <c r="I47" s="38"/>
+      <c r="J47" s="52"/>
+      <c r="K47" s="53"/>
+    </row>
+    <row r="48" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B49" s="29"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="31">
+      <c r="B48" s="45"/>
+      <c r="C48" s="45"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="47">
         <v>140</v>
       </c>
-      <c r="F49" s="32"/>
-      <c r="G49" s="33"/>
-      <c r="H49" s="23"/>
-      <c r="I49" s="24"/>
-      <c r="J49" s="18"/>
-      <c r="K49" s="19"/>
-    </row>
-    <row r="50" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F48" s="48"/>
+      <c r="G48" s="49"/>
+      <c r="H48" s="39"/>
+      <c r="I48" s="40"/>
+      <c r="J48" s="54"/>
+      <c r="K48" s="55"/>
+    </row>
+    <row r="49" spans="11:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K49" s="1"/>
+    </row>
+    <row r="50" spans="11:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="51" spans="11:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="K52" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="13">
+    <mergeCell ref="J47:K48"/>
+    <mergeCell ref="G30:G36"/>
+    <mergeCell ref="H47:I48"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="G22:G27"/>
     <mergeCell ref="A1:K2"/>
     <mergeCell ref="C8:J10"/>
-    <mergeCell ref="G15:G23"/>
-    <mergeCell ref="H15:H21"/>
-    <mergeCell ref="I15:I21"/>
-    <mergeCell ref="J48:K49"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="I15:I17"/>
     <mergeCell ref="A3:K6"/>
-    <mergeCell ref="H48:I49"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="G27:G33"/>
-    <mergeCell ref="H27:H31"/>
-    <mergeCell ref="I27:I31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="58" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>